<commit_message>
Finished up everything. Powerpoint is in this commit.
</commit_message>
<xml_diff>
--- a/SchoolData.xlsx
+++ b/SchoolData.xlsx
@@ -18,7 +18,7 @@
     <externalReference r:id="rId2"/>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1056,11 +1056,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="223162752"/>
-        <c:axId val="223159488"/>
+        <c:axId val="-1679391216"/>
+        <c:axId val="-1679386320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="223162752"/>
+        <c:axId val="-1679391216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1"/>
@@ -1118,12 +1118,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223159488"/>
+        <c:crossAx val="-1679386320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="223159488"/>
+        <c:axId val="-1679386320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1180,7 +1180,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223162752"/>
+        <c:crossAx val="-1679391216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1506,11 +1506,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="362668128"/>
-        <c:axId val="362668672"/>
+        <c:axId val="-1679398288"/>
+        <c:axId val="-1679386864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="362668128"/>
+        <c:axId val="-1679398288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1"/>
@@ -1568,12 +1568,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362668672"/>
+        <c:crossAx val="-1679386864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="362668672"/>
+        <c:axId val="-1679386864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1630,7 +1630,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362668128"/>
+        <c:crossAx val="-1679398288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2085,11 +2085,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="229786528"/>
-        <c:axId val="229783264"/>
+        <c:axId val="-1679385232"/>
+        <c:axId val="-1679390672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="229786528"/>
+        <c:axId val="-1679385232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2146,12 +2146,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229783264"/>
+        <c:crossAx val="-1679390672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="229783264"/>
+        <c:axId val="-1679390672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2208,7 +2208,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229786528"/>
+        <c:crossAx val="-1679385232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2534,11 +2534,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="229788160"/>
-        <c:axId val="229782720"/>
+        <c:axId val="-1679397200"/>
+        <c:axId val="-1679399920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="229788160"/>
+        <c:axId val="-1679397200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2595,12 +2595,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229782720"/>
+        <c:crossAx val="-1679399920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="229782720"/>
+        <c:axId val="-1679399920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2657,7 +2657,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229788160"/>
+        <c:crossAx val="-1679397200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2988,11 +2988,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="223165472"/>
-        <c:axId val="2107508528"/>
+        <c:axId val="-1679393392"/>
+        <c:axId val="-1679392848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="223165472"/>
+        <c:axId val="-1679393392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="60"/>
@@ -3050,12 +3050,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2107508528"/>
+        <c:crossAx val="-1679392848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2107508528"/>
+        <c:axId val="-1679392848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3112,7 +3112,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223165472"/>
+        <c:crossAx val="-1679393392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3451,11 +3451,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="20840656"/>
-        <c:axId val="20837392"/>
+        <c:axId val="-1679397744"/>
+        <c:axId val="-1679387408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="20840656"/>
+        <c:axId val="-1679397744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="60"/>
@@ -3513,12 +3513,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20837392"/>
+        <c:crossAx val="-1679387408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="20837392"/>
+        <c:axId val="-1679387408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3575,7 +3575,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20840656"/>
+        <c:crossAx val="-1679397744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3677,7 +3677,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3914,11 +3913,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="242815120"/>
-        <c:axId val="242816752"/>
+        <c:axId val="-1637938624"/>
+        <c:axId val="-1637947872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="242815120"/>
+        <c:axId val="-1637938624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3975,12 +3974,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242816752"/>
+        <c:crossAx val="-1637947872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="242816752"/>
+        <c:axId val="-1637947872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4037,7 +4036,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242815120"/>
+        <c:crossAx val="-1637938624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8724,7 +8723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="J85" sqref="J85"/>
     </sheetView>
   </sheetViews>
@@ -8812,7 +8811,7 @@
         <v>14</v>
       </c>
       <c r="N2">
-        <f>J2/K2</f>
+        <f t="shared" ref="N2:N15" si="0">J2/K2</f>
         <v>1.2857142857142858</v>
       </c>
       <c r="P2">
@@ -8822,7 +8821,7 @@
         <v>9</v>
       </c>
       <c r="T2">
-        <f>P2/Q2</f>
+        <f t="shared" ref="T2:T15" si="1">P2/Q2</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -8861,7 +8860,7 @@
         <v>15</v>
       </c>
       <c r="N3">
-        <f>J3/K3</f>
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="P3">
@@ -8871,7 +8870,7 @@
         <v>7</v>
       </c>
       <c r="T3">
-        <f>P3/Q3</f>
+        <f t="shared" si="1"/>
         <v>0.8571428571428571</v>
       </c>
     </row>
@@ -8910,7 +8909,7 @@
         <v>14</v>
       </c>
       <c r="N4">
-        <f>J4/K4</f>
+        <f t="shared" si="0"/>
         <v>1.2857142857142858</v>
       </c>
       <c r="P4">
@@ -8920,7 +8919,7 @@
         <v>5</v>
       </c>
       <c r="T4">
-        <f>P4/Q4</f>
+        <f t="shared" si="1"/>
         <v>1.6</v>
       </c>
     </row>
@@ -8959,7 +8958,7 @@
         <v>9</v>
       </c>
       <c r="N5">
-        <f>J5/K5</f>
+        <f t="shared" si="0"/>
         <v>2.6666666666666665</v>
       </c>
       <c r="P5">
@@ -8969,7 +8968,7 @@
         <v>4</v>
       </c>
       <c r="T5">
-        <f>P5/Q5</f>
+        <f t="shared" si="1"/>
         <v>2.25</v>
       </c>
     </row>
@@ -9008,7 +9007,7 @@
         <v>11</v>
       </c>
       <c r="N6">
-        <f>J6/K6</f>
+        <f t="shared" si="0"/>
         <v>2.1818181818181817</v>
       </c>
       <c r="P6">
@@ -9018,7 +9017,7 @@
         <v>3</v>
       </c>
       <c r="T6">
-        <f>P6/Q6</f>
+        <f t="shared" si="1"/>
         <v>3.3333333333333335</v>
       </c>
     </row>
@@ -9057,7 +9056,7 @@
         <v>14</v>
       </c>
       <c r="N7">
-        <f>J7/K7</f>
+        <f t="shared" si="0"/>
         <v>1.3571428571428572</v>
       </c>
       <c r="P7">
@@ -9067,7 +9066,7 @@
         <v>9</v>
       </c>
       <c r="T7">
-        <f>P7/Q7</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -9106,7 +9105,7 @@
         <v>8</v>
       </c>
       <c r="N8">
-        <f>J8/K8</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="P8">
@@ -9116,7 +9115,7 @@
         <v>7</v>
       </c>
       <c r="T8">
-        <f>P8/Q8</f>
+        <f t="shared" si="1"/>
         <v>0.8571428571428571</v>
       </c>
     </row>
@@ -9155,7 +9154,7 @@
         <v>19</v>
       </c>
       <c r="N9">
-        <f>J9/K9</f>
+        <f t="shared" si="0"/>
         <v>0.63157894736842102</v>
       </c>
       <c r="P9">
@@ -9165,7 +9164,7 @@
         <v>4</v>
       </c>
       <c r="T9">
-        <f>P9/Q9</f>
+        <f t="shared" si="1"/>
         <v>2.25</v>
       </c>
     </row>
@@ -9204,7 +9203,7 @@
         <v>11</v>
       </c>
       <c r="N10">
-        <f>J10/K10</f>
+        <f t="shared" si="0"/>
         <v>2.0909090909090908</v>
       </c>
       <c r="P10">
@@ -9214,7 +9213,7 @@
         <v>6</v>
       </c>
       <c r="T10">
-        <f>P10/Q10</f>
+        <f t="shared" si="1"/>
         <v>1.1666666666666667</v>
       </c>
     </row>
@@ -9253,7 +9252,7 @@
         <v>15</v>
       </c>
       <c r="N11">
-        <f>J11/K11</f>
+        <f t="shared" si="0"/>
         <v>1.1333333333333333</v>
       </c>
       <c r="P11">
@@ -9263,7 +9262,7 @@
         <v>2</v>
       </c>
       <c r="T11">
-        <f>P11/Q11</f>
+        <f t="shared" si="1"/>
         <v>5.5</v>
       </c>
     </row>
@@ -9302,7 +9301,7 @@
         <v>18</v>
       </c>
       <c r="N12">
-        <f>J12/K12</f>
+        <f t="shared" si="0"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="P12">
@@ -9312,7 +9311,7 @@
         <v>3</v>
       </c>
       <c r="T12">
-        <f>P12/Q12</f>
+        <f t="shared" si="1"/>
         <v>3.6666666666666665</v>
       </c>
     </row>
@@ -9351,7 +9350,7 @@
         <v>7</v>
       </c>
       <c r="N13">
-        <f>J13/K13</f>
+        <f t="shared" si="0"/>
         <v>3.5714285714285716</v>
       </c>
       <c r="P13">
@@ -9361,7 +9360,7 @@
         <v>9</v>
       </c>
       <c r="T13">
-        <f>P13/Q13</f>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -9400,7 +9399,7 @@
         <v>18</v>
       </c>
       <c r="N14">
-        <f>J14/K14</f>
+        <f t="shared" si="0"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="P14">
@@ -9410,7 +9409,7 @@
         <v>10</v>
       </c>
       <c r="T14">
-        <f>P14/Q14</f>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
     </row>
@@ -9449,7 +9448,7 @@
         <v>9</v>
       </c>
       <c r="N15">
-        <f>J15/K15</f>
+        <f t="shared" si="0"/>
         <v>2.7777777777777777</v>
       </c>
       <c r="P15">
@@ -9459,7 +9458,7 @@
         <v>3</v>
       </c>
       <c r="T15">
-        <f>P15/Q15</f>
+        <f t="shared" si="1"/>
         <v>3.6666666666666665</v>
       </c>
     </row>

</xml_diff>